<commit_message>
Check tests and update dependencies
</commit_message>
<xml_diff>
--- a/tests/Fable.exceljs.JsNativeTests/WriteTest.xlsx
+++ b/tests/Fable.exceljs.JsNativeTests/WriteTest.xlsx
@@ -405,7 +405,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1">
-        <v>45050.48714643519</v>
+        <v>40826.53333333333</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -416,7 +416,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="1">
-        <v>45050.48714643519</v>
+        <v>40826.53333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>